<commit_message>
Arreglado error diferent objects with same ID
</commit_message>
<xml_diff>
--- a/recursos/SistemasInformacionII.xlsx
+++ b/recursos/SistemasInformacionII.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Google Drive\UNIVERSIDAD\Curso 20-21\Sistemas de Información II\Practica 3\Este año\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco HDD 1TB Datos\grado en ingeniería informática\TERCER CURSO\7.SISTEMAS DE INFORMACION II\Practica\NominasSIS2\Prueba\NominasSIS2\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F76176F-6B44-4E86-96B0-63077BCD0AA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="6" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="672">
   <si>
     <t>Nombre</t>
   </si>
@@ -1172,15 +1171,9 @@
     <t>99558741836555551120</t>
   </si>
   <si>
-    <t>09548150L</t>
-  </si>
-  <si>
     <t>32541112811220000588</t>
   </si>
   <si>
-    <t>09548416X</t>
-  </si>
-  <si>
     <t>12548521518742146695</t>
   </si>
   <si>
@@ -1250,9 +1243,6 @@
     <t>65168874641561561500</t>
   </si>
   <si>
-    <t>09548295P</t>
-  </si>
-  <si>
     <t>36952365020014425254</t>
   </si>
   <si>
@@ -1295,9 +1285,6 @@
     <t>36585214290025478551</t>
   </si>
   <si>
-    <t>09785530J</t>
-  </si>
-  <si>
     <t>21651651812511133551</t>
   </si>
   <si>
@@ -1334,9 +1321,6 @@
     <t>X8996448K</t>
   </si>
   <si>
-    <t>09548827E</t>
-  </si>
-  <si>
     <t>66552211148855332200</t>
   </si>
   <si>
@@ -1431,9 +1415,6 @@
   </si>
   <si>
     <t>96431245118150005156</t>
-  </si>
-  <si>
-    <t>09458455Y</t>
   </si>
   <si>
     <t>25894363475485700145</t>
@@ -2066,7 +2047,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -2137,7 +2118,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2229,23 +2210,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2281,23 +2245,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2473,25 +2420,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2508,7 +2455,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2525,7 +2472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2542,7 +2489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2559,7 +2506,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2576,7 +2523,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2593,7 +2540,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2610,7 +2557,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2627,7 +2574,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2644,7 +2591,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2661,7 +2608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2678,7 +2625,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -2695,7 +2642,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2712,7 +2659,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -2729,7 +2676,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2746,7 +2693,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>15</v>
       </c>
@@ -2754,7 +2701,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>16</v>
       </c>
@@ -2762,7 +2709,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>17</v>
       </c>
@@ -2770,7 +2717,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>18</v>
       </c>
@@ -2780,23 +2727,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EF4386-161F-40EB-988F-578A9F806D0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="41.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="41.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2810,7 +2758,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12000</v>
       </c>
@@ -2824,7 +2772,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13000</v>
       </c>
@@ -2838,7 +2786,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14000</v>
       </c>
@@ -2852,7 +2800,7 @@
         <v>23.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15000</v>
       </c>
@@ -2866,7 +2814,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16000</v>
       </c>
@@ -2880,7 +2828,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>17000</v>
       </c>
@@ -2894,7 +2842,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18000</v>
       </c>
@@ -2908,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>19000</v>
       </c>
@@ -2916,7 +2864,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20000</v>
       </c>
@@ -2924,7 +2872,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>21000</v>
       </c>
@@ -2932,7 +2880,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22000</v>
       </c>
@@ -2940,7 +2888,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23000</v>
       </c>
@@ -2948,7 +2896,7 @@
         <v>13.65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>24000</v>
       </c>
@@ -2956,7 +2904,7 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25000</v>
       </c>
@@ -2964,7 +2912,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>26000</v>
       </c>
@@ -2972,7 +2920,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>27000</v>
       </c>
@@ -2980,7 +2928,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>28000</v>
       </c>
@@ -2988,7 +2936,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>29000</v>
       </c>
@@ -2996,7 +2944,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30000</v>
       </c>
@@ -3004,7 +2952,7 @@
         <v>17.25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31000</v>
       </c>
@@ -3012,7 +2960,7 @@
         <v>17.45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>32000</v>
       </c>
@@ -3020,7 +2968,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>33000</v>
       </c>
@@ -3028,7 +2976,7 @@
         <v>18.149999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>34000</v>
       </c>
@@ -3036,7 +2984,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>35000</v>
       </c>
@@ -3044,7 +2992,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>36000</v>
       </c>
@@ -3052,7 +3000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>37000</v>
       </c>
@@ -3060,7 +3008,7 @@
         <v>19.25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>38000</v>
       </c>
@@ -3068,7 +3016,7 @@
         <v>19.62</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>39000</v>
       </c>
@@ -3076,7 +3024,7 @@
         <v>19.96</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>40000</v>
       </c>
@@ -3084,7 +3032,7 @@
         <v>20.18</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>41000</v>
       </c>
@@ -3092,7 +3040,7 @@
         <v>20.52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>42000</v>
       </c>
@@ -3100,7 +3048,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>43000</v>
       </c>
@@ -3108,7 +3056,7 @@
         <v>21.12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>44000</v>
       </c>
@@ -3116,7 +3064,7 @@
         <v>21.45</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>45000</v>
       </c>
@@ -3124,7 +3072,7 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>46000</v>
       </c>
@@ -3132,7 +3080,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>47000</v>
       </c>
@@ -3140,7 +3088,7 @@
         <v>22.32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>48000</v>
       </c>
@@ -3148,7 +3096,7 @@
         <v>22.62</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>49000</v>
       </c>
@@ -3156,7 +3104,7 @@
         <v>22.92</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>50000</v>
       </c>
@@ -3164,7 +3112,7 @@
         <v>23.22</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>51000</v>
       </c>
@@ -3172,7 +3120,7 @@
         <v>23.52</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>52000</v>
       </c>
@@ -3180,7 +3128,7 @@
         <v>23.82</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>53000</v>
       </c>
@@ -3188,7 +3136,7 @@
         <v>24.12</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>54000</v>
       </c>
@@ -3196,7 +3144,7 @@
         <v>24.42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>55000</v>
       </c>
@@ -3204,7 +3152,7 @@
         <v>24.72</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>56000</v>
       </c>
@@ -3212,7 +3160,7 @@
         <v>25.02</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>57000</v>
       </c>
@@ -3220,7 +3168,7 @@
         <v>25.32</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>58000</v>
       </c>
@@ -3228,7 +3176,7 @@
         <v>25.62</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>59000</v>
       </c>
@@ -3236,7 +3184,7 @@
         <v>25.92</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>60000</v>
       </c>
@@ -3250,26 +3198,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="28.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="2" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="28.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3310,7 +3258,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -3339,19 +3287,19 @@
         <v>53</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="K2" t="s">
         <v>87</v>
       </c>
       <c r="L2" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="M2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -3380,19 +3328,19 @@
         <v>20</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="K3" t="s">
         <v>82</v>
       </c>
       <c r="L3" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="M3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3421,19 +3369,19 @@
         <v>53</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="K4" t="s">
         <v>366</v>
       </c>
       <c r="L4" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="M4" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -3462,19 +3410,19 @@
         <v>20</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="K5" t="s">
         <v>83</v>
       </c>
       <c r="L5" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="M5" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -3503,24 +3451,24 @@
         <v>20</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="K6" t="s">
         <v>359</v>
       </c>
       <c r="L6" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="M6" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="H7" s="4"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -3549,19 +3497,19 @@
         <v>53</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="K8" t="s">
         <v>84</v>
       </c>
       <c r="L8" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="M8" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>374</v>
       </c>
@@ -3590,19 +3538,19 @@
         <v>20</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="K9" t="s">
         <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="M9" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -3625,7 +3573,7 @@
         <v>54</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="I10" t="s">
         <v>53</v>
@@ -3637,13 +3585,13 @@
         <v>86</v>
       </c>
       <c r="L10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="M10" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -3666,25 +3614,25 @@
         <v>54</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="I11" t="s">
         <v>53</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="K11" t="s">
         <v>82</v>
       </c>
       <c r="L11" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="M11" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>376</v>
       </c>
@@ -3713,19 +3661,19 @@
         <v>53</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="K12" t="s">
         <v>363</v>
       </c>
       <c r="L12" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="M12" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>376</v>
       </c>
@@ -3754,19 +3702,19 @@
         <v>20</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="K13" t="s">
         <v>369</v>
       </c>
       <c r="L13" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="M13" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -3792,19 +3740,19 @@
         <v>20</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="K14" t="s">
         <v>85</v>
       </c>
       <c r="L14" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="M14" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -3833,19 +3781,19 @@
         <v>20</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="K15" t="s">
         <v>82</v>
       </c>
       <c r="L15" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="M15" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>374</v>
       </c>
@@ -3874,19 +3822,19 @@
         <v>20</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="K16" t="s">
         <v>368</v>
       </c>
       <c r="L16" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="M16" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>374</v>
       </c>
@@ -3915,19 +3863,19 @@
         <v>53</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K17" t="s">
         <v>82</v>
       </c>
       <c r="L17" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="M17" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>374</v>
       </c>
@@ -3956,19 +3904,19 @@
         <v>20</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="K18" t="s">
         <v>360</v>
       </c>
       <c r="L18" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="M18" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>374</v>
       </c>
@@ -3997,19 +3945,19 @@
         <v>53</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="K19" t="s">
         <v>362</v>
       </c>
       <c r="L19" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="M19" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -4038,19 +3986,19 @@
         <v>53</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="K20" t="s">
         <v>82</v>
       </c>
       <c r="L20" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="M20" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -4070,25 +4018,25 @@
         <v>81</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="I21" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="K21" t="s">
         <v>87</v>
       </c>
       <c r="L21" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="M21" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -4111,25 +4059,25 @@
         <v>352</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="I22" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="K22" t="s">
         <v>82</v>
       </c>
       <c r="L22" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="M22" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -4161,13 +4109,13 @@
         <v>84</v>
       </c>
       <c r="L23" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="M23" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -4190,25 +4138,25 @@
         <v>28</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="I24" t="s">
         <v>53</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="K24" t="s">
         <v>82</v>
       </c>
       <c r="L24" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="M24" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -4237,24 +4185,24 @@
         <v>53</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="K25" t="s">
         <v>83</v>
       </c>
       <c r="L25" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="M25" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="H26" s="4"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -4283,19 +4231,19 @@
         <v>53</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="K27" t="s">
         <v>82</v>
       </c>
       <c r="L27" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="M27" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -4324,19 +4272,19 @@
         <v>20</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="K28" t="s">
         <v>82</v>
       </c>
       <c r="L28" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="M28" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>374</v>
       </c>
@@ -4365,19 +4313,19 @@
         <v>53</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="K29" t="s">
         <v>372</v>
       </c>
       <c r="L29" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="M29" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -4406,19 +4354,19 @@
         <v>20</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="K30" t="s">
         <v>82</v>
       </c>
       <c r="L30" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="M30" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>374</v>
       </c>
@@ -4447,19 +4395,19 @@
         <v>20</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="K31" t="s">
         <v>82</v>
       </c>
       <c r="L31" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="M31" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -4488,19 +4436,19 @@
         <v>20</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="K32" t="s">
         <v>370</v>
       </c>
       <c r="L32" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="M32" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -4529,19 +4477,19 @@
         <v>53</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K33" t="s">
         <v>82</v>
       </c>
       <c r="L33" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="M33" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>376</v>
       </c>
@@ -4570,19 +4518,19 @@
         <v>53</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="K34" t="s">
         <v>365</v>
       </c>
       <c r="L34" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="M34" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -4611,19 +4559,19 @@
         <v>53</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="K35" t="s">
         <v>360</v>
       </c>
       <c r="L35" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="M35" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>374</v>
       </c>
@@ -4652,19 +4600,19 @@
         <v>53</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="K36" t="s">
         <v>83</v>
       </c>
       <c r="L36" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="M36" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -4687,25 +4635,25 @@
         <v>343</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I37" t="s">
         <v>20</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="K37" t="s">
         <v>83</v>
       </c>
       <c r="L37" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="M37" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>374</v>
       </c>
@@ -4734,19 +4682,19 @@
         <v>53</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="K38" t="s">
         <v>82</v>
       </c>
       <c r="L38" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="M38" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -4775,19 +4723,19 @@
         <v>53</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="K39" t="s">
         <v>82</v>
       </c>
       <c r="L39" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="M39" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -4816,19 +4764,19 @@
         <v>53</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K40" t="s">
         <v>82</v>
       </c>
       <c r="L40" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="M40" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>374</v>
       </c>
@@ -4857,19 +4805,19 @@
         <v>53</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="K41" t="s">
         <v>82</v>
       </c>
       <c r="L41" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="M41" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -4898,19 +4846,19 @@
         <v>53</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="K42" t="s">
         <v>86</v>
       </c>
       <c r="L42" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="M42" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -4933,25 +4881,25 @@
         <v>26</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I43" t="s">
         <v>53</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="K43" t="s">
         <v>82</v>
       </c>
       <c r="L43" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="M43" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -4980,19 +4928,19 @@
         <v>53</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="K44" t="s">
         <v>82</v>
       </c>
       <c r="L44" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="M44" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>376</v>
       </c>
@@ -5021,19 +4969,19 @@
         <v>53</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="K45" t="s">
         <v>82</v>
       </c>
       <c r="L45" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="M45" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -5062,19 +5010,19 @@
         <v>53</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="K46" t="s">
         <v>82</v>
       </c>
       <c r="L46" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="M46" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -5103,19 +5051,19 @@
         <v>20</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="K47" t="s">
         <v>82</v>
       </c>
       <c r="L47" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="M47" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -5135,7 +5083,7 @@
         <v>63</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I48" t="s">
         <v>20</v>
@@ -5147,13 +5095,13 @@
         <v>88</v>
       </c>
       <c r="L48" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="M48" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -5173,25 +5121,25 @@
         <v>65</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="I49" t="s">
         <v>20</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="K49" t="s">
         <v>83</v>
       </c>
       <c r="L49" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="M49" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -5220,19 +5168,19 @@
         <v>53</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="K50" t="s">
         <v>83</v>
       </c>
       <c r="L50" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="M50" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -5255,25 +5203,25 @@
         <v>21</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="I51" t="s">
         <v>20</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="K51" t="s">
         <v>82</v>
       </c>
       <c r="L51" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="M51" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -5302,19 +5250,19 @@
         <v>20</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="K52" t="s">
         <v>368</v>
       </c>
       <c r="L52" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="M52" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>376</v>
       </c>
@@ -5343,19 +5291,19 @@
         <v>20</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="K53" t="s">
         <v>82</v>
       </c>
       <c r="L53" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="M53" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>376</v>
       </c>
@@ -5384,19 +5332,19 @@
         <v>20</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="K54" t="s">
         <v>84</v>
       </c>
       <c r="L54" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="M54" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>376</v>
       </c>
@@ -5425,19 +5373,19 @@
         <v>53</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K55" t="s">
         <v>88</v>
       </c>
       <c r="L55" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="M55" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>98</v>
       </c>
@@ -5466,24 +5414,24 @@
         <v>20</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="K56" t="s">
         <v>82</v>
       </c>
       <c r="L56" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="M56" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="H57" s="4"/>
       <c r="L57"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -5506,7 +5454,7 @@
         <v>24</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I58" t="s">
         <v>20</v>
@@ -5518,13 +5466,13 @@
         <v>82</v>
       </c>
       <c r="L58" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="M58" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -5553,19 +5501,19 @@
         <v>53</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="K59" t="s">
         <v>82</v>
       </c>
       <c r="L59" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="M59" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>97</v>
       </c>
@@ -5594,19 +5542,19 @@
         <v>20</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K60" t="s">
         <v>82</v>
       </c>
       <c r="L60" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="M60" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>376</v>
       </c>
@@ -5635,19 +5583,19 @@
         <v>53</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="K61" t="s">
         <v>88</v>
       </c>
       <c r="L61" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="M61" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -5676,19 +5624,19 @@
         <v>20</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="K62" t="s">
         <v>82</v>
       </c>
       <c r="L62" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="M62" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -5717,19 +5665,19 @@
         <v>53</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="K63" t="s">
         <v>82</v>
       </c>
       <c r="L63" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="M63" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>376</v>
       </c>
@@ -5758,19 +5706,19 @@
         <v>20</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="K64" t="s">
         <v>82</v>
       </c>
       <c r="L64" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="M64" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -5799,19 +5747,19 @@
         <v>20</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="K65" t="s">
         <v>82</v>
       </c>
       <c r="L65" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="M65" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>97</v>
       </c>
@@ -5834,7 +5782,7 @@
         <v>91</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I66" t="s">
         <v>20</v>
@@ -5846,13 +5794,13 @@
         <v>82</v>
       </c>
       <c r="L66" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="M66" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>374</v>
       </c>
@@ -5875,25 +5823,25 @@
         <v>298</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I67" t="s">
         <v>53</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K67" t="s">
         <v>82</v>
       </c>
       <c r="L67" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="M67" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>376</v>
       </c>
@@ -5922,19 +5870,19 @@
         <v>20</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="K68" t="s">
         <v>82</v>
       </c>
       <c r="L68" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="M68" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>378</v>
       </c>
@@ -5963,19 +5911,19 @@
         <v>20</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K69" t="s">
         <v>82</v>
       </c>
       <c r="L69" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="M69" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>374</v>
       </c>
@@ -6004,19 +5952,19 @@
         <v>20</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="K70" t="s">
         <v>82</v>
       </c>
       <c r="L70" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="M70" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>97</v>
       </c>
@@ -6039,25 +5987,25 @@
         <v>25</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I71" t="s">
         <v>20</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K71" t="s">
         <v>82</v>
       </c>
       <c r="L71" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="M71" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>97</v>
       </c>
@@ -6086,19 +6034,19 @@
         <v>53</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K72" t="s">
         <v>372</v>
       </c>
       <c r="L72" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="M72" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>376</v>
       </c>
@@ -6121,25 +6069,25 @@
         <v>289</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="I73" t="s">
         <v>53</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K73" t="s">
         <v>82</v>
       </c>
       <c r="L73" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="M73" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>97</v>
       </c>
@@ -6168,19 +6116,19 @@
         <v>20</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K74" t="s">
         <v>82</v>
       </c>
       <c r="L74" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="M74" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>376</v>
       </c>
@@ -6209,19 +6157,19 @@
         <v>20</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K75" t="s">
         <v>82</v>
       </c>
       <c r="L75" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="M75" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>98</v>
       </c>
@@ -6250,24 +6198,24 @@
         <v>53</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K76" t="s">
         <v>364</v>
       </c>
       <c r="L76" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="M76" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D77" s="1"/>
       <c r="H77" s="4"/>
       <c r="L77"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>97</v>
       </c>
@@ -6300,13 +6248,13 @@
         <v>82</v>
       </c>
       <c r="L78" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="M78" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>376</v>
       </c>
@@ -6335,19 +6283,19 @@
         <v>53</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K79" t="s">
         <v>82</v>
       </c>
       <c r="L79" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="M79" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>97</v>
       </c>
@@ -6382,13 +6330,13 @@
         <v>82</v>
       </c>
       <c r="L80" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="M80" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>378</v>
       </c>
@@ -6417,19 +6365,19 @@
         <v>20</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K81" t="s">
         <v>86</v>
       </c>
       <c r="L81" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="M81" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>376</v>
       </c>
@@ -6458,19 +6406,19 @@
         <v>53</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K82" t="s">
         <v>82</v>
       </c>
       <c r="L82" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="M82" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>374</v>
       </c>
@@ -6503,13 +6451,13 @@
         <v>370</v>
       </c>
       <c r="L83" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="M83" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>376</v>
       </c>
@@ -6538,19 +6486,19 @@
         <v>20</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K84" t="s">
         <v>82</v>
       </c>
       <c r="L84" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="M84" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>378</v>
       </c>
@@ -6579,19 +6527,19 @@
         <v>53</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K85" t="s">
         <v>82</v>
       </c>
       <c r="L85" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="M85" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>378</v>
       </c>
@@ -6620,19 +6568,19 @@
         <v>53</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K86" t="s">
         <v>82</v>
       </c>
       <c r="L86" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="M86" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -6661,19 +6609,19 @@
         <v>20</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K87" t="s">
         <v>363</v>
       </c>
       <c r="L87" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="M87" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>378</v>
       </c>
@@ -6702,19 +6650,19 @@
         <v>20</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K88" t="s">
         <v>82</v>
       </c>
       <c r="L88" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="M88" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>378</v>
       </c>
@@ -6743,19 +6691,19 @@
         <v>20</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K89" t="s">
         <v>82</v>
       </c>
       <c r="L89" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="M89" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>374</v>
       </c>
@@ -6784,19 +6732,19 @@
         <v>20</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K90" t="s">
         <v>368</v>
       </c>
       <c r="L90" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="M90" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -6825,19 +6773,19 @@
         <v>53</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K91" t="s">
         <v>367</v>
       </c>
       <c r="L91" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="M91" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -6866,19 +6814,19 @@
         <v>20</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K92" t="s">
         <v>82</v>
       </c>
       <c r="L92" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="M92" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -6901,25 +6849,25 @@
         <v>27</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I93" t="s">
         <v>20</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K93" t="s">
         <v>82</v>
       </c>
       <c r="L93" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="M93" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -6942,25 +6890,25 @@
         <v>255</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I94" t="s">
         <v>20</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K94" t="s">
         <v>360</v>
       </c>
       <c r="L94" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="M94" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>376</v>
       </c>
@@ -6989,19 +6937,19 @@
         <v>20</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K95" t="s">
         <v>82</v>
       </c>
       <c r="L95" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="M95" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>378</v>
       </c>
@@ -7030,19 +6978,19 @@
         <v>20</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K96" t="s">
         <v>82</v>
       </c>
       <c r="L96" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="M96" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>378</v>
       </c>
@@ -7071,24 +7019,24 @@
         <v>20</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K97" t="s">
         <v>82</v>
       </c>
       <c r="L97" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="M97" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="H98" s="4"/>
       <c r="L98"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>378</v>
       </c>
@@ -7123,13 +7071,13 @@
         <v>361</v>
       </c>
       <c r="L99" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="M99" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>378</v>
       </c>
@@ -7152,25 +7100,25 @@
         <v>196</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I100" t="s">
         <v>20</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K100" t="s">
         <v>87</v>
       </c>
       <c r="L100" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="M100" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -7205,13 +7153,13 @@
         <v>363</v>
       </c>
       <c r="L101" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="M101" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>376</v>
       </c>
@@ -7246,13 +7194,13 @@
         <v>360</v>
       </c>
       <c r="L102" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="M102" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>98</v>
       </c>
@@ -7287,13 +7235,13 @@
         <v>362</v>
       </c>
       <c r="L103" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="M103" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>98</v>
       </c>
@@ -7328,10 +7276,10 @@
         <v>371</v>
       </c>
       <c r="L104" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="M104" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>